<commit_message>
modifications made to the excel file, it was missing some columns
</commit_message>
<xml_diff>
--- a/PDC-A1-Analysis.xlsx
+++ b/PDC-A1-Analysis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\6TH Semester\CSC-3075 Parallel And Distributed Computing\Labs\Asg-1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\junaid467\PDC\PDC-A1-1167-K_Means_Clustering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C9FD678B-0475-4E4F-B230-4D5FD54994AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEA0D6C2-7E5F-494A-A721-0C20126E9850}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15480" xr2:uid="{7B7D4387-B303-46F4-9A05-9562E969E02F}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="28800" windowHeight="15480" xr2:uid="{7B7D4387-B303-46F4-9A05-9562E969E02F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Parallel</t>
   </si>
@@ -59,19 +59,7 @@
     <t>AVERAGE</t>
   </si>
   <si>
-    <t>Compared to Sequential</t>
-  </si>
-  <si>
-    <t>Sum</t>
-  </si>
-  <si>
     <t>Average</t>
-  </si>
-  <si>
-    <t>Running Total</t>
-  </si>
-  <si>
-    <t>Count</t>
   </si>
   <si>
     <t>Static</t>
@@ -82,12 +70,15 @@
   <si>
     <t>Speedup</t>
   </si>
+  <si>
+    <t>Thread Analysis</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,6 +106,20 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -136,11 +141,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3855,10 +3864,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D817AAF2-3104-4B68-AC12-C98B0B438915}">
-  <dimension ref="A1:E272"/>
+  <dimension ref="A1:T272"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="74" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="Q25" sqref="Q25"/>
+      <selection activeCell="T29" sqref="T29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3868,10 +3877,15 @@
     <col min="3" max="3" width="16.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="2"/>
+    <col min="6" max="16" width="9.140625" style="2"/>
+    <col min="17" max="17" width="11.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.140625" style="2"/>
+    <col min="20" max="20" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -3887,8 +3901,13 @@
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="R1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -3904,8 +3923,17 @@
       <c r="E2" s="2">
         <v>2.8661140000000001</v>
       </c>
+      <c r="R2" s="1">
+        <v>4</v>
+      </c>
+      <c r="S2" s="1">
+        <v>8</v>
+      </c>
+      <c r="T2" s="1">
+        <v>12</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -3921,8 +3949,17 @@
       <c r="E3" s="2">
         <v>2.5460289999999999</v>
       </c>
+      <c r="R3" s="2">
+        <v>0.98955000000000004</v>
+      </c>
+      <c r="S3" s="2">
+        <v>0.67409200000000002</v>
+      </c>
+      <c r="T3" s="2">
+        <v>0.62112900000000004</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -3938,8 +3975,17 @@
       <c r="E4" s="2">
         <v>2.8596180000000002</v>
       </c>
+      <c r="R4" s="2">
+        <v>0.97959600000000002</v>
+      </c>
+      <c r="S4" s="2">
+        <v>0.80583800000000005</v>
+      </c>
+      <c r="T4" s="2">
+        <v>0.68840699999999999</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -3955,8 +4001,17 @@
       <c r="E5" s="2">
         <v>2.8723109999999998</v>
       </c>
+      <c r="R5" s="2">
+        <v>0.97959600000000002</v>
+      </c>
+      <c r="S5" s="2">
+        <v>0.60995299999999997</v>
+      </c>
+      <c r="T5" s="2">
+        <v>0.59116900000000006</v>
+      </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -3972,8 +4027,17 @@
       <c r="E6" s="2">
         <v>3.0437379999999998</v>
       </c>
+      <c r="R6" s="2">
+        <v>0.98004800000000003</v>
+      </c>
+      <c r="S6" s="2">
+        <v>0.61863900000000005</v>
+      </c>
+      <c r="T6" s="2">
+        <v>0.54764400000000002</v>
+      </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -3989,8 +4053,17 @@
       <c r="E7" s="2">
         <v>3.0291679999999999</v>
       </c>
+      <c r="R7" s="2">
+        <v>1.005169</v>
+      </c>
+      <c r="S7" s="2">
+        <v>0.66234899999999997</v>
+      </c>
+      <c r="T7" s="2">
+        <v>0.64939599999999997</v>
+      </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -4006,8 +4079,17 @@
       <c r="E8" s="2">
         <v>3.0201769999999999</v>
       </c>
+      <c r="R8" s="2">
+        <v>1.165956</v>
+      </c>
+      <c r="S8" s="2">
+        <v>0.68978899999999999</v>
+      </c>
+      <c r="T8" s="2">
+        <v>0.56184900000000004</v>
+      </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -4023,8 +4105,17 @@
       <c r="E9" s="2">
         <v>2.9155989999999998</v>
       </c>
+      <c r="R9" s="2">
+        <v>0.99114800000000003</v>
+      </c>
+      <c r="S9" s="2">
+        <v>0.62302999999999997</v>
+      </c>
+      <c r="T9" s="2">
+        <v>0.55396599999999996</v>
+      </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -4040,8 +4131,17 @@
       <c r="E10" s="2">
         <v>2.8786350000000001</v>
       </c>
+      <c r="R10" s="2">
+        <v>0.99605600000000005</v>
+      </c>
+      <c r="S10" s="2">
+        <v>0.84406899999999996</v>
+      </c>
+      <c r="T10" s="2">
+        <v>0.59214500000000003</v>
+      </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -4057,8 +4157,17 @@
       <c r="E11" s="2">
         <v>2.761101</v>
       </c>
+      <c r="R11" s="2">
+        <v>0.98483200000000004</v>
+      </c>
+      <c r="S11" s="2">
+        <v>0.92725000000000002</v>
+      </c>
+      <c r="T11" s="2">
+        <v>0.56433</v>
+      </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>6</v>
       </c>
@@ -4078,10 +4187,19 @@
         <f t="shared" si="0"/>
         <v>2.8792490000000002</v>
       </c>
+      <c r="R12" s="2">
+        <v>1.020416</v>
+      </c>
+      <c r="S12" s="2">
+        <v>0.79823900000000003</v>
+      </c>
+      <c r="T12" s="2">
+        <v>0.59398200000000001</v>
+      </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B13" s="3">
         <f>B12/B12</f>
@@ -4099,8 +4217,23 @@
         <f>B12/E12</f>
         <v>1.1864209035064353</v>
       </c>
+      <c r="Q13" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="R13" s="3">
+        <f>AVERAGE(R3:R12)</f>
+        <v>1.0092367</v>
+      </c>
+      <c r="S13" s="3">
+        <f t="shared" ref="S13:T13" si="1">AVERAGE(S3:S12)</f>
+        <v>0.72532479999999988</v>
+      </c>
+      <c r="T13" s="3">
+        <f t="shared" si="1"/>
+        <v>0.59640170000000003</v>
+      </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
     </row>
     <row r="269" spans="1:1" x14ac:dyDescent="0.25">
@@ -4115,15 +4248,18 @@
     </row>
     <row r="271" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A271" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="272" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A272" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="R1:T1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
updated the report pdf
</commit_message>
<xml_diff>
--- a/PDC-A1-Analysis.xlsx
+++ b/PDC-A1-Analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\junaid467\PDC\PDC-A1-1167-K_Means_Clustering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEA0D6C2-7E5F-494A-A721-0C20126E9850}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBD8E600-9E99-4261-89CE-DB9E7B375154}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="28800" windowHeight="15480" xr2:uid="{7B7D4387-B303-46F4-9A05-9562E969E02F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7B7D4387-B303-46F4-9A05-9562E969E02F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Parallel</t>
   </si>
@@ -72,6 +72,27 @@
   </si>
   <si>
     <t>Thread Analysis</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>100k</t>
+  </si>
+  <si>
+    <t>500k</t>
+  </si>
+  <si>
+    <t>Chunk Analysis(Static)</t>
+  </si>
+  <si>
+    <t>Chunk Analysis(Dynamic)</t>
+  </si>
+  <si>
+    <t>2k</t>
+  </si>
+  <si>
+    <t>20k</t>
   </si>
 </sst>
 </file>
@@ -141,15 +162,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3864,10 +3887,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D817AAF2-3104-4B68-AC12-C98B0B438915}">
-  <dimension ref="A1:T272"/>
+  <dimension ref="A1:AC272"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="74" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="T29" sqref="T29"/>
+      <selection activeCell="B1" sqref="B1:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3882,10 +3905,12 @@
     <col min="18" max="18" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="9.140625" style="2"/>
     <col min="20" max="20" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="9.140625" style="2"/>
+    <col min="21" max="22" width="9.140625" style="2"/>
+    <col min="23" max="23" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="25.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:29" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -3901,13 +3926,24 @@
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="V1" s="7"/>
+      <c r="W1" s="7"/>
+      <c r="Z1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA1" s="7"/>
+      <c r="AB1" s="7"/>
+      <c r="AC1" s="7"/>
     </row>
-    <row r="2" spans="1:20" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -3932,8 +3968,26 @@
       <c r="T2" s="1">
         <v>12</v>
       </c>
+      <c r="U2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -3958,8 +4012,26 @@
       <c r="T3" s="2">
         <v>0.62112900000000004</v>
       </c>
+      <c r="U3" s="2">
+        <v>0.55310099999999995</v>
+      </c>
+      <c r="V3" s="2">
+        <v>0.65168400000000004</v>
+      </c>
+      <c r="W3" s="2">
+        <v>2.6363500000000002</v>
+      </c>
+      <c r="Z3" s="2">
+        <v>0.56407499999999999</v>
+      </c>
+      <c r="AA3" s="2">
+        <v>1.046397</v>
+      </c>
+      <c r="AB3" s="2">
+        <v>0.65960200000000002</v>
+      </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -3984,8 +4056,26 @@
       <c r="T4" s="2">
         <v>0.68840699999999999</v>
       </c>
+      <c r="U4" s="2">
+        <v>0.66796699999999998</v>
+      </c>
+      <c r="V4" s="2">
+        <v>0.69090200000000002</v>
+      </c>
+      <c r="W4" s="2">
+        <v>1.705927</v>
+      </c>
+      <c r="Z4" s="2">
+        <v>0.479601</v>
+      </c>
+      <c r="AA4" s="2">
+        <v>0.88029400000000002</v>
+      </c>
+      <c r="AB4" s="2">
+        <v>0.70581499999999997</v>
+      </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -4010,8 +4100,26 @@
       <c r="T5" s="2">
         <v>0.59116900000000006</v>
       </c>
+      <c r="U5" s="2">
+        <v>0.73206899999999997</v>
+      </c>
+      <c r="V5" s="2">
+        <v>0.71185600000000004</v>
+      </c>
+      <c r="W5" s="2">
+        <v>1.6528130000000001</v>
+      </c>
+      <c r="Z5" s="2">
+        <v>0.57695799999999997</v>
+      </c>
+      <c r="AA5" s="2">
+        <v>1.0357080000000001</v>
+      </c>
+      <c r="AB5" s="2">
+        <v>0.67049499999999995</v>
+      </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -4036,8 +4144,26 @@
       <c r="T6" s="2">
         <v>0.54764400000000002</v>
       </c>
+      <c r="U6" s="2">
+        <v>0.68669199999999997</v>
+      </c>
+      <c r="V6" s="2">
+        <v>0.69811299999999998</v>
+      </c>
+      <c r="W6" s="2">
+        <v>1.6074649999999999</v>
+      </c>
+      <c r="Z6" s="2">
+        <v>0.63431099999999996</v>
+      </c>
+      <c r="AA6" s="2">
+        <v>1.054648</v>
+      </c>
+      <c r="AB6" s="2">
+        <v>0.79444700000000001</v>
+      </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -4062,8 +4188,26 @@
       <c r="T7" s="2">
         <v>0.64939599999999997</v>
       </c>
+      <c r="U7" s="2">
+        <v>0.59839900000000001</v>
+      </c>
+      <c r="V7" s="2">
+        <v>0.687338</v>
+      </c>
+      <c r="W7" s="2">
+        <v>1.653788</v>
+      </c>
+      <c r="Z7" s="2">
+        <v>0.530192</v>
+      </c>
+      <c r="AA7" s="2">
+        <v>0.55704100000000001</v>
+      </c>
+      <c r="AB7" s="2">
+        <v>0.68912099999999998</v>
+      </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -4088,8 +4232,26 @@
       <c r="T8" s="2">
         <v>0.56184900000000004</v>
       </c>
+      <c r="U8" s="2">
+        <v>0.72872700000000001</v>
+      </c>
+      <c r="V8" s="2">
+        <v>0.69798300000000002</v>
+      </c>
+      <c r="W8" s="2">
+        <v>1.675405</v>
+      </c>
+      <c r="Z8" s="2">
+        <v>0.64984399999999998</v>
+      </c>
+      <c r="AA8" s="2">
+        <v>0.57006699999999999</v>
+      </c>
+      <c r="AB8" s="2">
+        <v>0.72543599999999997</v>
+      </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -4114,8 +4276,26 @@
       <c r="T9" s="2">
         <v>0.55396599999999996</v>
       </c>
+      <c r="U9" s="2">
+        <v>0.74073599999999995</v>
+      </c>
+      <c r="V9" s="2">
+        <v>0.730182</v>
+      </c>
+      <c r="W9" s="2">
+        <v>1.663754</v>
+      </c>
+      <c r="Z9" s="2">
+        <v>0.82967599999999997</v>
+      </c>
+      <c r="AA9" s="2">
+        <v>0.73188799999999998</v>
+      </c>
+      <c r="AB9" s="2">
+        <v>0.62317500000000003</v>
+      </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -4140,8 +4320,26 @@
       <c r="T10" s="2">
         <v>0.59214500000000003</v>
       </c>
+      <c r="U10" s="2">
+        <v>0.56140299999999999</v>
+      </c>
+      <c r="V10" s="2">
+        <v>0.70450299999999999</v>
+      </c>
+      <c r="W10" s="2">
+        <v>1.6377619999999999</v>
+      </c>
+      <c r="Z10" s="2">
+        <v>0.56317300000000003</v>
+      </c>
+      <c r="AA10" s="2">
+        <v>0.57795700000000005</v>
+      </c>
+      <c r="AB10" s="2">
+        <v>0.71948000000000001</v>
+      </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -4166,8 +4364,26 @@
       <c r="T11" s="2">
         <v>0.56433</v>
       </c>
+      <c r="U11" s="2">
+        <v>0.61216400000000004</v>
+      </c>
+      <c r="V11" s="2">
+        <v>0.69301800000000002</v>
+      </c>
+      <c r="W11" s="2">
+        <v>1.581904</v>
+      </c>
+      <c r="Z11" s="2">
+        <v>0.84920099999999998</v>
+      </c>
+      <c r="AA11" s="2">
+        <v>0.6351</v>
+      </c>
+      <c r="AB11" s="2">
+        <v>0.693971</v>
+      </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>6</v>
       </c>
@@ -4196,8 +4412,26 @@
       <c r="T12" s="2">
         <v>0.59398200000000001</v>
       </c>
+      <c r="U12" s="2">
+        <v>0.58741200000000005</v>
+      </c>
+      <c r="V12" s="2">
+        <v>0.84129399999999999</v>
+      </c>
+      <c r="W12" s="2">
+        <v>1.664733</v>
+      </c>
+      <c r="Z12" s="2">
+        <v>0.51833399999999996</v>
+      </c>
+      <c r="AA12" s="2">
+        <v>0.60865000000000002</v>
+      </c>
+      <c r="AB12" s="2">
+        <v>0.69115099999999996</v>
+      </c>
     </row>
-    <row r="13" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>10</v>
       </c>
@@ -4217,7 +4451,7 @@
         <f>B12/E12</f>
         <v>1.1864209035064353</v>
       </c>
-      <c r="Q13" s="5" t="s">
+      <c r="Q13" s="4" t="s">
         <v>7</v>
       </c>
       <c r="R13" s="3">
@@ -4225,15 +4459,41 @@
         <v>1.0092367</v>
       </c>
       <c r="S13" s="3">
-        <f t="shared" ref="S13:T13" si="1">AVERAGE(S3:S12)</f>
+        <f t="shared" ref="S13:AB13" si="1">AVERAGE(S3:S12)</f>
         <v>0.72532479999999988</v>
       </c>
       <c r="T13" s="3">
         <f t="shared" si="1"/>
         <v>0.59640170000000003</v>
       </c>
+      <c r="U13" s="3">
+        <f t="shared" si="1"/>
+        <v>0.64686699999999997</v>
+      </c>
+      <c r="V13" s="3">
+        <f t="shared" si="1"/>
+        <v>0.71068730000000002</v>
+      </c>
+      <c r="W13" s="3">
+        <f t="shared" si="1"/>
+        <v>1.7479900999999998</v>
+      </c>
+      <c r="X13" s="3"/>
+      <c r="Y13" s="3"/>
+      <c r="Z13" s="3">
+        <f t="shared" si="1"/>
+        <v>0.61953649999999993</v>
+      </c>
+      <c r="AA13" s="3">
+        <f t="shared" si="1"/>
+        <v>0.76977499999999988</v>
+      </c>
+      <c r="AB13" s="3">
+        <f t="shared" si="1"/>
+        <v>0.69726929999999998</v>
+      </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
     </row>
     <row r="269" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>